<commit_message>
ppm CO and NO2
</commit_message>
<xml_diff>
--- a/form calibration sensor.xlsx
+++ b/form calibration sensor.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHIO\Documents\Projects EC\breakout_MICS4514\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2FD718-1126-4092-BDFE-1EC6010079B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38958DD3-BB2A-46AE-9CEC-9E2B36FEED3B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="510" windowWidth="13305" windowHeight="11820" xr2:uid="{976D1E1A-5E4F-4282-BCFD-16D726701E86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{976D1E1A-5E4F-4282-BCFD-16D726701E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>ppm</t>
   </si>
@@ -108,12 +109,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -122,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -157,31 +161,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>CO DATASHEET</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -195,7 +174,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -226,21 +205,21 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ppm</c:v>
+                  <c:v>Rs/R0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="6"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -249,28 +228,28 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
-              <a:ln w="9525" cap="rnd">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="0"/>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.5317288967911269E-2"/>
-                  <c:y val="-0.48191610324327833"/>
+                  <c:x val="4.3331583552055991E-2"/>
+                  <c:y val="-0.38608231262758824"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -279,7 +258,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
                           <a:schemeClr val="tx1">
                             <a:lumMod val="65000"/>
@@ -292,14 +271,17 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
-                      <a:t>y = 971.43e</a:t>
+                      <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+                      <a:t>y = -0.116ln(x) + 0.8102</a:t>
                     </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+                    </a:br>
                     <a:r>
-                      <a:rPr lang="en-US" sz="2400" b="1" baseline="30000"/>
-                      <a:t>-9.177x</a:t>
+                      <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+                      <a:t>R² = 0.9872</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" sz="2400" b="1"/>
+                    <a:endParaRPr lang="en-US" sz="2000" b="1"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -316,7 +298,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -333,74 +315,82 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$3:$A$11</c:f>
+              <c:f>Hoja1!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.47</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$B$11</c:f>
+              <c:f>Hoja1!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1000</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,7 +398,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B1E5-4D2C-B21F-2BC71E2CDE0B}"/>
+              <c16:uniqueId val="{00000000-894A-4B77-B9F3-A7798635EBB4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -420,11 +410,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="498754184"/>
-        <c:axId val="498757136"/>
+        <c:axId val="617785528"/>
+        <c:axId val="617786184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="498754184"/>
+        <c:axId val="617785528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,8 +443,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -466,7 +456,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -481,12 +471,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="498757136"/>
+        <c:crossAx val="617786184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="498757136"/>
+        <c:axId val="617786184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -514,9 +504,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -543,7 +533,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="498754184"/>
+        <c:crossAx val="617785528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -557,11 +547,441 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rs/R0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-MX"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja2!$A$3:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>850</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja2!$B$3:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E2BB-49FA-8B5D-D574C47E1E6B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="619921784"/>
+        <c:axId val="623551952"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="619921784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="623551952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="623551952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619921784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -632,8 +1052,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -644,7 +1104,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -660,25 +1120,25 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -690,7 +1150,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -698,11 +1158,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -734,45 +1194,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -784,26 +1234,22 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -833,13 +1279,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -849,7 +1297,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -858,135 +1306,205 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -996,77 +1514,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1075,13 +1523,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1095,26 +1544,27 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1131,7 +1581,84 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1139,6 +1666,445 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1146,8 +2112,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1156,23 +2128,64 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BAA76F1-34FB-4571-8838-9ACC1ACB7D64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C9EFE5C-193C-4B4D-9D58-91C0CBDF3584}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3686813C-53DE-4FF2-BF6E-DBA00D6E1246}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1492,8 +2505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE7F840-A868-4038-994E-397D2F5CDFFC}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,232 +2516,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="G1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>0.47</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.33750000000000002</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="G3" s="2">
-        <v>3</v>
-      </c>
-      <c r="H3" s="2">
-        <v>11</v>
-      </c>
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>0.7</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2">
-        <v>1.35E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>5</v>
-      </c>
-      <c r="G4" s="2">
-        <v>6</v>
-      </c>
-      <c r="H4" s="2">
-        <v>30</v>
-      </c>
+        <v>0.6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>0.6</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="G5" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>40</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>0.5</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="G6" s="2">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2">
-        <v>45</v>
-      </c>
+        <v>0.4</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>0.4</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2">
-        <v>40</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="G7" s="2">
-        <v>30</v>
-      </c>
-      <c r="H7" s="2">
-        <v>90</v>
-      </c>
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>0.3</v>
+        <v>150</v>
       </c>
       <c r="B8" s="2">
-        <v>80</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="G8" s="2">
-        <v>35</v>
-      </c>
-      <c r="H8" s="2">
-        <v>100</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>0.2</v>
+        <v>350</v>
       </c>
       <c r="B9" s="2">
-        <v>150</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="G9" s="2">
-        <v>200</v>
-      </c>
-      <c r="H9" s="2">
-        <v>230</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>0.1</v>
+        <v>1000</v>
       </c>
       <c r="B10" s="2">
-        <v>350</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="G10" s="2">
-        <v>350</v>
-      </c>
-      <c r="H10" s="2">
-        <v>300</v>
-      </c>
+        <v>3.1E-2</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>3.1E-2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="G11" s="2">
-        <v>700</v>
-      </c>
-      <c r="H11" s="2">
-        <v>400</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="G12" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H12" s="2">
-        <v>480</v>
-      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="G13" s="2">
-        <v>2000</v>
-      </c>
-      <c r="H13" s="2">
-        <v>650</v>
-      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="G14" s="2">
-        <v>3000</v>
-      </c>
-      <c r="H14" s="2">
-        <v>750</v>
-      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="G15" s="2">
-        <v>4000</v>
-      </c>
-      <c r="H15" s="2">
-        <v>850</v>
-      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.25">
@@ -1736,12 +2661,148 @@
       <c r="H17" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44BAC4-3708-40A7-80D3-71EA55D4CA79}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>40</v>
+      </c>
+      <c r="B5" s="2">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>90</v>
+      </c>
+      <c r="B7" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>100</v>
+      </c>
+      <c r="B8" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>230</v>
+      </c>
+      <c r="B9" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>300</v>
+      </c>
+      <c r="B10" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>400</v>
+      </c>
+      <c r="B11" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>480</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>650</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>750</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>850</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change equations and datasheet
</commit_message>
<xml_diff>
--- a/form calibration sensor.xlsx
+++ b/form calibration sensor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHIO\Documents\Projects EC\breakout_MICS4514\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38958DD3-BB2A-46AE-9CEC-9E2B36FEED3B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F259D016-5CB3-480F-AF28-305F18EB11B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{976D1E1A-5E4F-4282-BCFD-16D726701E86}"/>
+    <workbookView xWindow="8280" yWindow="540" windowWidth="12690" windowHeight="11820" xr2:uid="{976D1E1A-5E4F-4282-BCFD-16D726701E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>ppm</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>NO2</t>
+  </si>
+  <si>
+    <t>http://files.manylabs.org/datasheets/MICS-4514.pdf</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -105,11 +108,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -123,10 +137,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -205,14 +222,16 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rs/R0</c:v>
+                  <c:v>ppm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -242,14 +261,14 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.3331583552055991E-2"/>
-                  <c:y val="-0.38608231262758824"/>
+                  <c:x val="-9.7739282589676291E-2"/>
+                  <c:y val="-0.4269061679790026"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -271,17 +290,21 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
-                      <a:t>y = -0.116ln(x) + 0.8102</a:t>
+                      <a:rPr lang="en-US" sz="2400" baseline="0"/>
+                      <a:t>y = 4.4138x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2400" baseline="30000"/>
+                      <a:t>-1.178</a:t>
                     </a:r>
                     <a:br>
-                      <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+                      <a:rPr lang="en-US" sz="2400" baseline="0"/>
                     </a:br>
                     <a:r>
-                      <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
-                      <a:t>R² = 0.9872</a:t>
+                      <a:rPr lang="en-US" sz="2400" baseline="0"/>
+                      <a:t>R² = 0.9982</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" sz="2000" b="1"/>
+                    <a:endParaRPr lang="en-US" sz="2400"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -315,82 +338,104 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$3:$A$10</c:f>
+              <c:f>Hoja1!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>1.1000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>150</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>350</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1000</c:v>
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$B$10</c:f>
+              <c:f>Hoja1!$B$3:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,7 +443,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-894A-4B77-B9F3-A7798635EBB4}"/>
+              <c16:uniqueId val="{00000000-CD3C-4EB9-82AF-7B8D9C376CF9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -410,11 +455,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="617785528"/>
-        <c:axId val="617786184"/>
+        <c:axId val="564724896"/>
+        <c:axId val="576102232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="617785528"/>
+        <c:axId val="564724896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,12 +516,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617786184"/>
+        <c:crossAx val="576102232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="617786184"/>
+        <c:axId val="576102232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -533,7 +578,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617785528"/>
+        <c:crossAx val="564724896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -637,7 +682,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -648,7 +693,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rs/R0</c:v>
+                  <c:v>ppm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -677,6 +722,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -724,104 +783,116 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja2!$A$3:$A$15</c:f>
+              <c:f>Hoja2!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>650</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>850</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja2!$B$3:$B$15</c:f>
+              <c:f>Hoja2!$B$3:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>350</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E2BB-49FA-8B5D-D574C47E1E6B}"/>
+              <c16:uniqueId val="{00000000-E4A9-4465-8206-5E51D2E34A91}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -833,11 +904,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="619921784"/>
-        <c:axId val="623551952"/>
+        <c:axId val="576098624"/>
+        <c:axId val="576097640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="619921784"/>
+        <c:axId val="576098624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,12 +965,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="623551952"/>
+        <c:crossAx val="576097640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="623551952"/>
+        <c:axId val="576097640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +1027,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="619921784"/>
+        <c:crossAx val="576098624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2129,22 +2200,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BAA76F1-34FB-4571-8838-9ACC1ACB7D64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09D3E6AF-34E8-4012-A099-BBF6EED71ED6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2169,23 +2240,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2">
+        <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3686813C-53DE-4FF2-BF6E-DBA00D6E1246}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B0421BB-A3C4-421A-AE7E-480E03B4A6F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2503,10 +2574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE7F840-A868-4038-994E-397D2F5CDFFC}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,15 +2591,15 @@
         <v>2</v>
       </c>
       <c r="B1" s="4"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -2537,10 +2608,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="B3" s="2">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2549,10 +2620,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2561,104 +2632,130 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>20</v>
+        <v>1.5</v>
       </c>
       <c r="B5" s="2">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>40</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B6" s="2">
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>80</v>
+        <v>0.9</v>
       </c>
       <c r="B7" s="2">
-        <v>0.3</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>150</v>
+        <v>0.8</v>
       </c>
       <c r="B8" s="2">
-        <v>0.2</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>350</v>
+        <v>0.7</v>
       </c>
       <c r="B9" s="2">
-        <v>0.1</v>
+        <v>7</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>1000</v>
+        <v>0.6</v>
       </c>
       <c r="B10" s="2">
-        <v>3.1E-2</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="B12" s="2">
+        <v>30</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>50</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>100</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="B15" s="2">
+        <v>300</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2672,130 +2769,167 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44BAC4-3708-40A7-80D3-71EA55D4CA79}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="B12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>30</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>40</v>
-      </c>
-      <c r="B5" s="2">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>45</v>
-      </c>
-      <c r="B6" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>90</v>
-      </c>
-      <c r="B7" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>100</v>
-      </c>
-      <c r="B8" s="2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>230</v>
-      </c>
-      <c r="B9" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>300</v>
-      </c>
-      <c r="B10" s="2">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>400</v>
-      </c>
-      <c r="B11" s="2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>480</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>650</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>750</v>
-      </c>
-      <c r="B14" s="2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>850</v>
-      </c>
-      <c r="B15" s="2">
-        <v>4000</v>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shape of edge cuts
</commit_message>
<xml_diff>
--- a/form calibration sensor.xlsx
+++ b/form calibration sensor.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHIO\Documents\Projects EC\breakout_MICS4514\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F259D016-5CB3-480F-AF28-305F18EB11B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF76479A-5C96-40FC-AED0-DD87C16A5C05}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="540" windowWidth="12690" windowHeight="11820" xr2:uid="{976D1E1A-5E4F-4282-BCFD-16D726701E86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{976D1E1A-5E4F-4282-BCFD-16D726701E86}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="CO" sheetId="1" r:id="rId1"/>
+    <sheet name="NO2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>ppm</t>
   </si>
@@ -40,17 +40,34 @@
     <t>NO2</t>
   </si>
   <si>
-    <t>http://files.manylabs.org/datasheets/MICS-4514.pdf</t>
+    <t>https://www.wcf.com/hoja-de-informaci%C3%B3n-sobre-el-mon%C3%B3xido-de-carbono-co</t>
+  </si>
+  <si>
+    <t>https://www.sgxsensortech.com/content/uploads/2014/08/0278_Datasheet-MiCS-4514.pdf</t>
+  </si>
+  <si>
+    <t>DATASHEET 2:</t>
+  </si>
+  <si>
+    <t>Documento referencia ppm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,8 +137,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -134,20 +152,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -218,7 +235,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$2</c:f>
+              <c:f>CO!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -262,13 +279,41 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.7739282589676291E-2"/>
-                  <c:y val="-0.4269061679790026"/>
+                  <c:x val="1.3788495188101487E-2"/>
+                  <c:y val="-0.31903579760863227"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -290,21 +335,21 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr lang="en-US" sz="2400" baseline="0"/>
-                      <a:t>y = 4.4138x</a:t>
+                      <a:rPr lang="en-US" sz="3600" b="1" baseline="0"/>
+                      <a:t>y = 4.3873x</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="2400" baseline="30000"/>
-                      <a:t>-1.178</a:t>
+                      <a:rPr lang="en-US" sz="3600" b="1" baseline="30000"/>
+                      <a:t>-1.188</a:t>
                     </a:r>
                     <a:br>
-                      <a:rPr lang="en-US" sz="2400" baseline="0"/>
+                      <a:rPr lang="en-US" sz="3600" b="1" baseline="0"/>
                     </a:br>
                     <a:r>
-                      <a:rPr lang="en-US" sz="2400" baseline="0"/>
-                      <a:t>R² = 0.9982</a:t>
+                      <a:rPr lang="en-US" sz="3600" b="1" baseline="0"/>
+                      <a:t>R² = 0.9997</a:t>
                     </a:r>
-                    <a:endParaRPr lang="en-US" sz="2400"/>
+                    <a:endParaRPr lang="en-US" sz="3600" b="1"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -340,50 +385,44 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$3:$A$16</c:f>
+              <c:f>CO!$A$4:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.4</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.19</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.03</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
@@ -391,10 +430,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$3:$B$16</c:f>
+              <c:f>CO!$B$4:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -402,39 +441,33 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
@@ -443,7 +476,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CD3C-4EB9-82AF-7B8D9C376CF9}"/>
+              <c16:uniqueId val="{00000000-82A7-49C7-9BDD-1659BB19138B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -455,11 +488,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="564724896"/>
-        <c:axId val="576102232"/>
+        <c:axId val="505612328"/>
+        <c:axId val="294362752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="564724896"/>
+        <c:axId val="505612328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,12 +549,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="576102232"/>
+        <c:crossAx val="294362752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="576102232"/>
+        <c:axId val="294362752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -578,7 +611,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="564724896"/>
+        <c:crossAx val="505612328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -689,7 +722,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja2!$B$2</c:f>
+              <c:f>'NO2'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -783,7 +816,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja2!$A$3:$A$17</c:f>
+              <c:f>'NO2'!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -837,7 +870,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja2!$B$3:$B$17</c:f>
+              <c:f>'NO2'!$B$3:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2200,22 +2233,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:colOff>752475</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09D3E6AF-34E8-4012-A099-BBF6EED71ED6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F35B56E-F75E-4E3E-BDEF-6C2AA265863F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2574,10 +2607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE7F840-A868-4038-994E-397D2F5CDFFC}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A2:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2586,202 +2619,164 @@
     <col min="6" max="6" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3.5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="B12" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="B13" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="B14" s="2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="B7" s="2">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="B8" s="2">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>7</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>0.6</v>
-      </c>
-      <c r="B10" s="2">
-        <v>8</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="B11" s="2">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="B12" s="2">
-        <v>30</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="B13" s="2">
-        <v>50</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="B14" s="2">
-        <v>100</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="B15" s="2">
-        <v>300</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="G1:H1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D20" r:id="rId1" xr:uid="{50C8953C-93A1-4790-B7CD-7C9C0D2356C2}"/>
+    <hyperlink ref="D19" r:id="rId2" xr:uid="{3A7C9CFB-B704-49CF-AB49-167CECA2667E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44BAC4-3708-40A7-80D3-71EA55D4CA79}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2796,7 +2791,7 @@
       <c r="A3" s="2">
         <v>0.65</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="4">
         <v>0.01</v>
       </c>
       <c r="C3" s="1"/>
@@ -2918,7 +2913,7 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>40</v>
       </c>
@@ -2927,16 +2922,19 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F25">
-        <v>0</v>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C21" r:id="rId1" xr:uid="{948D39B3-8E08-4F3C-A27B-746B01DD5972}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>